<commit_message>
update name student from database
</commit_message>
<xml_diff>
--- a/file_excell/Student_Add.xlsx
+++ b/file_excell/Student_Add.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProjectStudentSKRU_NEW\file_excell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA3C1D1-C87B-4D5C-A0DC-37EB5FD975B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD7388FE-18C1-4AA6-B459-187D7DC10468}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{79D0B335-3B00-4AA3-BD32-79853FA32513}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>รหัสนักศึกษา</t>
   </si>
   <si>
-    <t>ชื่อ - นามสกุล</t>
-  </si>
-  <si>
     <t>คำอธิบายรหัสสาขาวิชา</t>
   </si>
   <si>
@@ -51,6 +48,15 @@
   </si>
   <si>
     <t>วิทยาการคอมพิวเตอร์</t>
+  </si>
+  <si>
+    <t>คำนำหน้า</t>
+  </si>
+  <si>
+    <t>ชื่อ</t>
+  </si>
+  <si>
+    <t>นามสุกล</t>
   </si>
 </sst>
 </file>
@@ -410,53 +416,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9FE214-0CAB-4857-84F0-5EC369000B8F}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="F2" t="s">
+    <row r="4" spans="1:9">
+      <c r="H4">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="I4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>